<commit_message>
Added Extent Reporter Java and working fine
</commit_message>
<xml_diff>
--- a/Selenium/testData/MLM.xlsx
+++ b/Selenium/testData/MLM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="21">
   <si>
     <t>Country</t>
   </si>
@@ -65,10 +65,16 @@
     <t>RunMode</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Skipped</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>Passed</t>
   </si>
   <si>
     <t>Failed</t>
@@ -111,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="161">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,27 +126,797 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -173,7 +949,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="87">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="2"/>
@@ -185,8 +961,86 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="104" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="106" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="110" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="112" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="116" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="118" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="122" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="124" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="128" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="130" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="132" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="134" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="136" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="138" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="140" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="142" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="144" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="146" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="148" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="150" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="152" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="154" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="156" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="158" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="160" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
@@ -549,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,15 +1458,63 @@
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s" s="8">
+      <c r="G4" t="s" s="86">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>